<commit_message>
Upload updated version of well index
</commit_message>
<xml_diff>
--- a/CellProfiler_OutputHandling/WellGeneIndexList.xlsx
+++ b/CellProfiler_OutputHandling/WellGeneIndexList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uio-my.sharepoint.com/personal/kristerv_uio_no/Documents/Papers - writings and comments/Screening Paper/Scripts and templates/CellProfiler_output_treatment/CellProfiler_OutputTreatment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uio-my.sharepoint.com/personal/kristerv_uio_no/Documents/Papers - writings and comments/Screening Paper/Scripts and templates/CellProfiler_output_treatment/CellProfiler_OutputHandling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="266" documentId="11_DC8ED11DA743F1B8C22264720F85A1E563A4FC5D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F64AF67-6A4C-4766-8A75-75A4670C1E7A}"/>
+  <xr:revisionPtr revIDLastSave="267" documentId="11_DC8ED11DA743F1B8C22264720F85A1E563A4FC5D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA9FD5B4-CAD5-47E9-A087-52C38B818615}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="10710" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -12600,9 +12600,6 @@
   </si>
   <si>
     <t>dnaAN346D, Chloramphenicol</t>
-  </si>
-  <si>
-    <t>hdaF100V, Tetracyclin</t>
   </si>
   <si>
     <t>mutD5zae, Tetracyclin</t>
@@ -12840,6 +12837,9 @@
       </rPr>
       <t>Kanamycin</t>
     </r>
+  </si>
+  <si>
+    <t>hdaF85V, Tetracyclin</t>
   </si>
 </sst>
 </file>
@@ -13226,10 +13226,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BM386"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16471,7 +16471,7 @@
         <v>4045</v>
       </c>
       <c r="V32" t="s">
-        <v>4186</v>
+        <v>4250</v>
       </c>
       <c r="W32" t="s">
         <v>4045</v>
@@ -16582,7 +16582,7 @@
         <v>4046</v>
       </c>
       <c r="V33" t="s">
-        <v>4187</v>
+        <v>4186</v>
       </c>
       <c r="W33" t="s">
         <v>4046</v>
@@ -16693,7 +16693,7 @@
         <v>4047</v>
       </c>
       <c r="V34" t="s">
-        <v>4188</v>
+        <v>4187</v>
       </c>
       <c r="W34" t="s">
         <v>4047</v>
@@ -18891,7 +18891,7 @@
         <v>4051</v>
       </c>
       <c r="V54" t="s">
-        <v>4193</v>
+        <v>4192</v>
       </c>
       <c r="W54" t="s">
         <v>4051</v>
@@ -19006,7 +19006,7 @@
         <v>4052</v>
       </c>
       <c r="V55" t="s">
-        <v>4194</v>
+        <v>4193</v>
       </c>
       <c r="W55" t="s">
         <v>4052</v>
@@ -19121,7 +19121,7 @@
         <v>4053</v>
       </c>
       <c r="V56" t="s">
-        <v>4195</v>
+        <v>4194</v>
       </c>
       <c r="W56" t="s">
         <v>4053</v>
@@ -19236,7 +19236,7 @@
         <v>4054</v>
       </c>
       <c r="V57" t="s">
-        <v>4196</v>
+        <v>4195</v>
       </c>
       <c r="W57" t="s">
         <v>4054</v>
@@ -21384,7 +21384,7 @@
         <v>4059</v>
       </c>
       <c r="V76" t="s">
-        <v>4197</v>
+        <v>4196</v>
       </c>
       <c r="W76" t="s">
         <v>4059</v>
@@ -21497,7 +21497,7 @@
         <v>4060</v>
       </c>
       <c r="V77" t="s">
-        <v>4198</v>
+        <v>4197</v>
       </c>
       <c r="W77" t="s">
         <v>4060</v>
@@ -21612,7 +21612,7 @@
         <v>4061</v>
       </c>
       <c r="V78" t="s">
-        <v>4199</v>
+        <v>4198</v>
       </c>
       <c r="W78" t="s">
         <v>4061</v>
@@ -21727,7 +21727,7 @@
         <v>4062</v>
       </c>
       <c r="V79" t="s">
-        <v>4228</v>
+        <v>4227</v>
       </c>
       <c r="W79" t="s">
         <v>4062</v>
@@ -21842,7 +21842,7 @@
         <v>4063</v>
       </c>
       <c r="V80" t="s">
-        <v>4237</v>
+        <v>4236</v>
       </c>
       <c r="W80" t="s">
         <v>4063</v>
@@ -21957,7 +21957,7 @@
         <v>4064</v>
       </c>
       <c r="V81" t="s">
-        <v>4238</v>
+        <v>4237</v>
       </c>
       <c r="W81" t="s">
         <v>4064</v>
@@ -24102,7 +24102,7 @@
         <v>4068</v>
       </c>
       <c r="V100" t="s">
-        <v>4200</v>
+        <v>4199</v>
       </c>
       <c r="W100" t="s">
         <v>4068</v>
@@ -24215,7 +24215,7 @@
         <v>4069</v>
       </c>
       <c r="V101" t="s">
-        <v>4201</v>
+        <v>4200</v>
       </c>
       <c r="W101" t="s">
         <v>4069</v>
@@ -24329,7 +24329,7 @@
         <v>4070</v>
       </c>
       <c r="V102" t="s">
-        <v>4202</v>
+        <v>4201</v>
       </c>
       <c r="W102" t="s">
         <v>4070</v>
@@ -24443,7 +24443,7 @@
         <v>4071</v>
       </c>
       <c r="V103" t="s">
-        <v>4229</v>
+        <v>4228</v>
       </c>
       <c r="W103" t="s">
         <v>4071</v>
@@ -24557,7 +24557,7 @@
         <v>4072</v>
       </c>
       <c r="V104" t="s">
-        <v>4239</v>
+        <v>4238</v>
       </c>
       <c r="W104" t="s">
         <v>4072</v>
@@ -26817,7 +26817,7 @@
         <v>4077</v>
       </c>
       <c r="V124" t="s">
-        <v>4203</v>
+        <v>4202</v>
       </c>
       <c r="W124" t="s">
         <v>4077</v>
@@ -26930,7 +26930,7 @@
         <v>4078</v>
       </c>
       <c r="V125" t="s">
-        <v>4204</v>
+        <v>4203</v>
       </c>
       <c r="W125" t="s">
         <v>4078</v>
@@ -27046,7 +27046,7 @@
         <v>4079</v>
       </c>
       <c r="V126" t="s">
-        <v>4205</v>
+        <v>4204</v>
       </c>
       <c r="W126" t="s">
         <v>4079</v>
@@ -27162,7 +27162,7 @@
         <v>4080</v>
       </c>
       <c r="V127" t="s">
-        <v>4230</v>
+        <v>4229</v>
       </c>
       <c r="W127" t="s">
         <v>4080</v>
@@ -27278,7 +27278,7 @@
         <v>4081</v>
       </c>
       <c r="V128" t="s">
-        <v>4240</v>
+        <v>4239</v>
       </c>
       <c r="W128" t="s">
         <v>4081</v>
@@ -29575,7 +29575,7 @@
         <v>4086</v>
       </c>
       <c r="V148" t="s">
-        <v>4206</v>
+        <v>4205</v>
       </c>
       <c r="W148" t="s">
         <v>4086</v>
@@ -29690,7 +29690,7 @@
         <v>4087</v>
       </c>
       <c r="V149" t="s">
-        <v>4207</v>
+        <v>4206</v>
       </c>
       <c r="W149" t="s">
         <v>4087</v>
@@ -29806,7 +29806,7 @@
         <v>4088</v>
       </c>
       <c r="V150" t="s">
-        <v>4205</v>
+        <v>4204</v>
       </c>
       <c r="W150" t="s">
         <v>4088</v>
@@ -29922,7 +29922,7 @@
         <v>4089</v>
       </c>
       <c r="V151" t="s">
-        <v>4231</v>
+        <v>4230</v>
       </c>
       <c r="W151" t="s">
         <v>4089</v>
@@ -30038,7 +30038,7 @@
         <v>4090</v>
       </c>
       <c r="V152" t="s">
-        <v>4249</v>
+        <v>4248</v>
       </c>
       <c r="W152" t="s">
         <v>4090</v>
@@ -32307,7 +32307,7 @@
         <v>4095</v>
       </c>
       <c r="V172" t="s">
-        <v>4208</v>
+        <v>4207</v>
       </c>
       <c r="W172" t="s">
         <v>4095</v>
@@ -32420,7 +32420,7 @@
         <v>4096</v>
       </c>
       <c r="V173" t="s">
-        <v>4250</v>
+        <v>4249</v>
       </c>
       <c r="W173" t="s">
         <v>4096</v>
@@ -32534,7 +32534,7 @@
         <v>4097</v>
       </c>
       <c r="V174" t="s">
-        <v>4209</v>
+        <v>4208</v>
       </c>
       <c r="W174" t="s">
         <v>4097</v>
@@ -32648,7 +32648,7 @@
         <v>4098</v>
       </c>
       <c r="V175" t="s">
-        <v>4232</v>
+        <v>4231</v>
       </c>
       <c r="W175" t="s">
         <v>4098</v>
@@ -32762,7 +32762,7 @@
         <v>4099</v>
       </c>
       <c r="V176" t="s">
-        <v>4241</v>
+        <v>4240</v>
       </c>
       <c r="W176" t="s">
         <v>4099</v>
@@ -34476,7 +34476,7 @@
         <v>305</v>
       </c>
       <c r="V191" t="s">
-        <v>4189</v>
+        <v>4188</v>
       </c>
       <c r="W191" t="s">
         <v>305</v>
@@ -35019,7 +35019,7 @@
         <v>4104</v>
       </c>
       <c r="V196" t="s">
-        <v>4210</v>
+        <v>4209</v>
       </c>
       <c r="W196" t="s">
         <v>4104</v>
@@ -35132,7 +35132,7 @@
         <v>4105</v>
       </c>
       <c r="V197" t="s">
-        <v>4211</v>
+        <v>4210</v>
       </c>
       <c r="W197" t="s">
         <v>4105</v>
@@ -35246,7 +35246,7 @@
         <v>4106</v>
       </c>
       <c r="V198" t="s">
-        <v>4209</v>
+        <v>4208</v>
       </c>
       <c r="W198" t="s">
         <v>4106</v>
@@ -35360,7 +35360,7 @@
         <v>4107</v>
       </c>
       <c r="V199" t="s">
-        <v>4233</v>
+        <v>4232</v>
       </c>
       <c r="W199" t="s">
         <v>4107</v>
@@ -35474,7 +35474,7 @@
         <v>4108</v>
       </c>
       <c r="V200" t="s">
-        <v>4242</v>
+        <v>4241</v>
       </c>
       <c r="W200" t="s">
         <v>4108</v>
@@ -37731,7 +37731,7 @@
         <v>4113</v>
       </c>
       <c r="V220" t="s">
-        <v>4212</v>
+        <v>4211</v>
       </c>
       <c r="W220" t="s">
         <v>4113</v>
@@ -37844,7 +37844,7 @@
         <v>4114</v>
       </c>
       <c r="V221" t="s">
-        <v>4213</v>
+        <v>4212</v>
       </c>
       <c r="W221" t="s">
         <v>4114</v>
@@ -37958,7 +37958,7 @@
         <v>4115</v>
       </c>
       <c r="V222" t="s">
-        <v>4214</v>
+        <v>4213</v>
       </c>
       <c r="W222" t="s">
         <v>4115</v>
@@ -38072,7 +38072,7 @@
         <v>4116</v>
       </c>
       <c r="V223" t="s">
-        <v>4234</v>
+        <v>4233</v>
       </c>
       <c r="W223" t="s">
         <v>4116</v>
@@ -38186,7 +38186,7 @@
         <v>4117</v>
       </c>
       <c r="V224" t="s">
-        <v>4243</v>
+        <v>4242</v>
       </c>
       <c r="W224" t="s">
         <v>4117</v>
@@ -39325,7 +39325,7 @@
         <v>373</v>
       </c>
       <c r="V234" t="s">
-        <v>4190</v>
+        <v>4189</v>
       </c>
       <c r="W234" t="s">
         <v>373</v>
@@ -40443,7 +40443,7 @@
         <v>4122</v>
       </c>
       <c r="V244" t="s">
-        <v>4215</v>
+        <v>4214</v>
       </c>
       <c r="W244" t="s">
         <v>4122</v>
@@ -40556,7 +40556,7 @@
         <v>4123</v>
       </c>
       <c r="V245" t="s">
-        <v>4216</v>
+        <v>4215</v>
       </c>
       <c r="W245" t="s">
         <v>4123</v>
@@ -40670,7 +40670,7 @@
         <v>4124</v>
       </c>
       <c r="V246" t="s">
-        <v>4217</v>
+        <v>4216</v>
       </c>
       <c r="W246" t="s">
         <v>4124</v>
@@ -40784,7 +40784,7 @@
         <v>4125</v>
       </c>
       <c r="V247" t="s">
-        <v>4235</v>
+        <v>4234</v>
       </c>
       <c r="W247" t="s">
         <v>4125</v>
@@ -40898,7 +40898,7 @@
         <v>4126</v>
       </c>
       <c r="V248" t="s">
-        <v>4244</v>
+        <v>4243</v>
       </c>
       <c r="W248" t="s">
         <v>4126</v>
@@ -43155,7 +43155,7 @@
         <v>4139</v>
       </c>
       <c r="V268" t="s">
-        <v>4218</v>
+        <v>4217</v>
       </c>
       <c r="W268" t="s">
         <v>4139</v>
@@ -43268,7 +43268,7 @@
         <v>4131</v>
       </c>
       <c r="V269" t="s">
-        <v>4219</v>
+        <v>4218</v>
       </c>
       <c r="W269" t="s">
         <v>4131</v>
@@ -43382,7 +43382,7 @@
         <v>4132</v>
       </c>
       <c r="V270" t="s">
-        <v>4220</v>
+        <v>4219</v>
       </c>
       <c r="W270" t="s">
         <v>4132</v>
@@ -43496,7 +43496,7 @@
         <v>4133</v>
       </c>
       <c r="V271" t="s">
-        <v>4236</v>
+        <v>4235</v>
       </c>
       <c r="W271" t="s">
         <v>4133</v>
@@ -43610,7 +43610,7 @@
         <v>4134</v>
       </c>
       <c r="V272" t="s">
-        <v>4245</v>
+        <v>4244</v>
       </c>
       <c r="W272" t="s">
         <v>4134</v>
@@ -43949,7 +43949,7 @@
         <v>4137</v>
       </c>
       <c r="V275" t="s">
-        <v>4191</v>
+        <v>4190</v>
       </c>
       <c r="W275" t="s">
         <v>4137</v>
@@ -45855,7 +45855,7 @@
         <v>4140</v>
       </c>
       <c r="V292" t="s">
-        <v>4221</v>
+        <v>4220</v>
       </c>
       <c r="W292" t="s">
         <v>4140</v>
@@ -45968,7 +45968,7 @@
         <v>4141</v>
       </c>
       <c r="V293" t="s">
-        <v>4222</v>
+        <v>4221</v>
       </c>
       <c r="W293" t="s">
         <v>4141</v>
@@ -46082,7 +46082,7 @@
         <v>4142</v>
       </c>
       <c r="V294" t="s">
-        <v>4223</v>
+        <v>4222</v>
       </c>
       <c r="W294" t="s">
         <v>4142</v>
@@ -46307,7 +46307,7 @@
         <v>4144</v>
       </c>
       <c r="V296" t="s">
-        <v>4246</v>
+        <v>4245</v>
       </c>
       <c r="W296" t="s">
         <v>4144</v>
@@ -48555,7 +48555,7 @@
         <v>4149</v>
       </c>
       <c r="V316" t="s">
-        <v>4224</v>
+        <v>4223</v>
       </c>
       <c r="W316" t="s">
         <v>4149</v>
@@ -48668,7 +48668,7 @@
         <v>4150</v>
       </c>
       <c r="V317" t="s">
-        <v>4225</v>
+        <v>4224</v>
       </c>
       <c r="W317" t="s">
         <v>4150</v>
@@ -49004,7 +49004,7 @@
         <v>4153</v>
       </c>
       <c r="V320" t="s">
-        <v>4247</v>
+        <v>4246</v>
       </c>
       <c r="W320" t="s">
         <v>4153</v>
@@ -51254,7 +51254,7 @@
         <v>4158</v>
       </c>
       <c r="V340" t="s">
-        <v>4226</v>
+        <v>4225</v>
       </c>
       <c r="W340" t="s">
         <v>4158</v>
@@ -51368,7 +51368,7 @@
         <v>4159</v>
       </c>
       <c r="V341" t="s">
-        <v>4227</v>
+        <v>4226</v>
       </c>
       <c r="W341" t="s">
         <v>4159</v>
@@ -51704,7 +51704,7 @@
         <v>4162</v>
       </c>
       <c r="V344" t="s">
-        <v>4248</v>
+        <v>4247</v>
       </c>
       <c r="W344" t="s">
         <v>4162</v>
@@ -53171,7 +53171,7 @@
         <v>573</v>
       </c>
       <c r="V357" t="s">
-        <v>4192</v>
+        <v>4191</v>
       </c>
       <c r="W357" t="s">
         <v>573</v>

</xml_diff>